<commit_message>
Added PasswordRecovery test Added new class: PasswordRecoveryPage
</commit_message>
<xml_diff>
--- a/STD/STD.xlsx
+++ b/STD/STD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afik\IdeaProjects\FinalProj\STD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21999CE6-AB17-4B00-BAD1-55B1E0282751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3D17CF-3E38-4314-AA24-748D0628C14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test design" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="192">
   <si>
     <t>Environment</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Login failed-password or email incorrect notification</t>
-  </si>
-  <si>
-    <t>Enter a valid password</t>
   </si>
   <si>
     <t>enter invalid email address</t>
@@ -616,6 +613,12 @@
   </si>
   <si>
     <t>Sign up-Test selector options</t>
+  </si>
+  <si>
+    <t>Enter an valid password</t>
+  </si>
+  <si>
+    <t>Test shopping cart recovery</t>
   </si>
 </sst>
 </file>
@@ -631,7 +634,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -698,8 +701,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -707,20 +716,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -735,6 +756,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1032,374 +1071,409 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="17">
+        <v>1</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="I3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17">
+        <v>2</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="I4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17">
+        <v>3</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="I5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="17">
+        <v>4</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="I6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17">
+        <v>5</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17">
+        <v>6</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17">
+        <v>7</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="17">
+        <v>8</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="18">
+        <v>9</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="18"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="18">
+        <v>10</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="18">
+        <v>10</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="18">
+        <v>11</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="18">
+        <v>12</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="18">
+        <v>13</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="18">
+        <v>14</v>
+      </c>
+      <c r="D19" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="18">
+        <v>15</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="18">
+        <v>16</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="18">
+        <v>17</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="18">
+        <v>18</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="18">
+        <v>19</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="18">
+        <v>20</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="B27" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="18">
+        <v>21</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="18"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="18">
+        <v>22</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" s="18"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+    </row>
+    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
+      <c r="B30" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="18">
+        <v>23</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18">
+        <v>24</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18">
+        <v>25</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18">
+        <v>26</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="4"/>
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16">
-        <v>12</v>
-      </c>
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19">
-        <v>14</v>
-      </c>
-      <c r="D19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20">
-        <v>15</v>
-      </c>
-      <c r="D20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21">
-        <v>16</v>
-      </c>
-      <c r="D21" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22">
-        <v>17</v>
-      </c>
-      <c r="D22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23">
-        <v>18</v>
-      </c>
-      <c r="D23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24">
-        <v>19</v>
-      </c>
-      <c r="D24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25">
-        <v>20</v>
-      </c>
-      <c r="D25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
-      <c r="B27" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="C27">
-        <v>21</v>
-      </c>
-      <c r="D27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="14"/>
-      <c r="C28">
-        <v>22</v>
-      </c>
-      <c r="D28" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
-      <c r="B30" t="s">
-        <v>135</v>
-      </c>
-      <c r="C30">
-        <v>23</v>
-      </c>
-      <c r="D30" t="s">
-        <v>172</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C31">
-        <v>24</v>
-      </c>
-      <c r="D31" t="s">
-        <v>173</v>
-      </c>
-      <c r="E31" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C32">
-        <v>25</v>
-      </c>
-      <c r="D32" t="s">
-        <v>176</v>
-      </c>
-      <c r="E32" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C33">
-        <v>26</v>
-      </c>
-      <c r="D33" t="s">
-        <v>177</v>
-      </c>
-      <c r="E33" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
+      <c r="C35" s="18">
+        <v>27</v>
+      </c>
+      <c r="D35" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="C35">
-        <v>27</v>
-      </c>
-      <c r="D35" t="s">
-        <v>180</v>
-      </c>
+      <c r="E35" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1417,32 +1491,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FF29FE-4C4A-4C54-B037-6F39A5D60650}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="110.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="110.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -1456,7 +1530,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3">
         <v>2</v>
@@ -1468,7 +1542,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4">
         <v>3</v>
@@ -1477,7 +1551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5">
         <v>4</v>
@@ -1489,7 +1563,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6">
         <v>5</v>
@@ -1498,7 +1572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7">
         <v>6</v>
@@ -1507,7 +1581,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8">
         <v>7</v>
@@ -1519,7 +1593,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9">
         <v>8</v>
@@ -1531,7 +1605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10">
         <v>9</v>
@@ -1543,13 +1617,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>2</v>
       </c>
@@ -1563,7 +1637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13">
         <v>2</v>
@@ -1575,7 +1649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14">
         <v>3</v>
@@ -1584,7 +1658,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15">
         <v>4</v>
@@ -1596,13 +1670,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>3</v>
       </c>
@@ -1616,7 +1690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18">
         <v>2</v>
@@ -1628,7 +1702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19">
         <v>3</v>
@@ -1637,7 +1711,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20">
         <v>4</v>
@@ -1649,13 +1723,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>4</v>
       </c>
@@ -1669,7 +1743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23">
         <v>2</v>
@@ -1681,7 +1755,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24">
         <v>3</v>
@@ -1690,7 +1764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25">
         <v>4</v>
@@ -1702,7 +1776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26">
         <v>5</v>
@@ -1714,13 +1788,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>5</v>
       </c>
@@ -1734,7 +1808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29">
         <v>2</v>
@@ -1746,7 +1820,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30">
         <v>3</v>
@@ -1755,7 +1829,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31">
         <v>4</v>
@@ -1764,7 +1838,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32">
         <v>5</v>
@@ -1776,13 +1850,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>6</v>
       </c>
@@ -1796,7 +1870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35">
         <v>2</v>
@@ -1808,26 +1882,26 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36">
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37">
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
       <c r="B38">
         <v>5</v>
       </c>
@@ -1838,13 +1912,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>7</v>
       </c>
@@ -1858,7 +1932,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41">
         <v>2</v>
@@ -1870,25 +1944,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42">
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43">
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="B44">
         <v>5</v>
@@ -1900,13 +1974,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>8</v>
       </c>
@@ -1920,7 +1994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
       <c r="B47">
         <v>2</v>
@@ -1932,57 +2006,57 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
       <c r="B48">
         <v>3</v>
       </c>
       <c r="C48" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" t="s">
         <v>44</v>
       </c>
-      <c r="D48" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
       <c r="B49">
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
       <c r="B50">
         <v>5</v>
       </c>
       <c r="C50" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
       <c r="B51">
         <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="15">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="14">
         <v>9</v>
       </c>
       <c r="B53">
@@ -1995,8 +2069,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="15"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
       <c r="B54">
         <v>2</v>
       </c>
@@ -2007,57 +2081,57 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="15"/>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="14"/>
       <c r="B55">
         <v>3</v>
       </c>
       <c r="C55" t="s">
+        <v>43</v>
+      </c>
+      <c r="D55" t="s">
         <v>44</v>
       </c>
-      <c r="D55" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="15"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
       <c r="B56">
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="15"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
       <c r="B57">
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="15"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="14"/>
       <c r="B58">
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="15">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="14">
         <v>10</v>
       </c>
       <c r="B60">
@@ -2070,8 +2144,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="15"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
       <c r="B61">
         <v>2</v>
       </c>
@@ -2082,8 +2156,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="15"/>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="14"/>
       <c r="B62">
         <v>3</v>
       </c>
@@ -2091,8 +2165,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="15"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
       <c r="B63">
         <v>4</v>
       </c>
@@ -2103,44 +2177,44 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="15"/>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
       <c r="B64">
         <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="15"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
       <c r="B65">
         <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="15"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
       <c r="B66">
         <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="15"/>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="14"/>
       <c r="B67">
         <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="15"/>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2150,10 +2224,10 @@
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A60:A68"/>
     <mergeCell ref="A28:A32"/>
-    <mergeCell ref="A34:A37"/>
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="A46:A51"/>
     <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A34:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2168,29 +2242,29 @@
       <selection activeCell="A12" sqref="A12:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
         <v>10</v>
       </c>
       <c r="B2">
@@ -2203,101 +2277,101 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
         <v>66</v>
       </c>
-      <c r="D11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
         <v>11</v>
       </c>
       <c r="B13">
@@ -2310,101 +2384,101 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
       <c r="B15">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
       <c r="B16">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
       <c r="B17">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
       <c r="B18">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
       <c r="B19">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
       <c r="B20">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
       <c r="B21">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
       <c r="B22">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
         <v>12</v>
       </c>
       <c r="B24">
@@ -2417,94 +2491,94 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
       <c r="B26">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
       <c r="B27">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
       <c r="B28">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
       <c r="B29">
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
       <c r="B30">
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
       <c r="B31">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
       <c r="B32">
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="15"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
       <c r="B33">
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2528,513 +2602,513 @@
       <selection activeCell="A17" sqref="A17:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
         <v>14</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="100.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
         <v>82</v>
       </c>
-      <c r="D6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
         <v>84</v>
       </c>
-      <c r="D8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" t="s">
         <v>94</v>
       </c>
-      <c r="D16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
         <v>15</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
       <c r="B20">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
         <v>16</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
       <c r="B24">
         <v>3</v>
       </c>
       <c r="C24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
         <v>17</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
       <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
       <c r="B28">
         <v>3</v>
       </c>
       <c r="C28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
         <v>18</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
       <c r="B31">
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
       <c r="B32">
         <v>3</v>
       </c>
       <c r="C32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
         <v>19</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="15"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
       <c r="B35">
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
       <c r="B36">
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="15"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
       <c r="B37">
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
       <c r="B38">
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
       <c r="B39">
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
       <c r="B40">
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
       <c r="B41">
         <v>8</v>
       </c>
       <c r="C41" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" t="s">
         <v>115</v>
       </c>
-      <c r="D41" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="15"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
       <c r="B42">
         <v>9</v>
       </c>
       <c r="C42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" t="s">
         <v>111</v>
       </c>
-      <c r="D42" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="15"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
       <c r="B43">
         <v>10</v>
       </c>
       <c r="C43" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" t="s">
         <v>113</v>
       </c>
-      <c r="D43" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="15"/>
+    </row>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
       <c r="B44">
         <v>11</v>
       </c>
       <c r="C44" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="15">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
         <v>20</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="15"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
       <c r="B47">
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="15"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
       <c r="B48">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="15"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
       <c r="B49">
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="15"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
       <c r="B50">
         <v>5</v>
       </c>
       <c r="C50" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -3062,29 +3136,29 @@
       <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>21</v>
       </c>
@@ -3092,46 +3166,46 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3147,178 +3221,178 @@
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
         <v>23</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" t="s">
         <v>136</v>
       </c>
-      <c r="D3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" t="s">
         <v>139</v>
       </c>
-      <c r="D4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" t="s">
         <v>141</v>
       </c>
-      <c r="D5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" t="s">
         <v>143</v>
       </c>
-      <c r="D6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="15">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
         <v>24</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" t="s">
         <v>151</v>
       </c>
-      <c r="D12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
       <c r="B15">
         <v>5</v>
       </c>
@@ -3326,191 +3400,191 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
       <c r="B16">
         <v>6</v>
       </c>
       <c r="C16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
       <c r="B17">
         <v>7</v>
       </c>
       <c r="C17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" t="s">
         <v>158</v>
       </c>
-      <c r="D17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
       <c r="B18">
         <v>8</v>
       </c>
       <c r="C18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" t="s">
         <v>160</v>
       </c>
-      <c r="D18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
       <c r="B19">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
         <v>25</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" t="s">
         <v>163</v>
       </c>
-      <c r="D21" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
       <c r="B25">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D25" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
       <c r="B26">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
       <c r="B27">
         <v>7</v>
       </c>
       <c r="C27" t="s">
+        <v>168</v>
+      </c>
+      <c r="D27" t="s">
         <v>169</v>
       </c>
-      <c r="D27" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
         <v>26</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" t="s">
         <v>163</v>
       </c>
-      <c r="D29" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
       <c r="B31">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
       <c r="B32">
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="15"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
       <c r="B33">
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D33" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3535,49 +3609,49 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="14">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
         <v>27</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" t="s">
         <v>182</v>
-      </c>
-      <c r="D3" t="s">
-        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split login and Sign up
</commit_message>
<xml_diff>
--- a/STD/STD.xlsx
+++ b/STD/STD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afik\IdeaProjects\FinalProj\STD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3D17CF-3E38-4314-AA24-748D0628C14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{024D8448-2608-47EA-94D7-F5BA6D119EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,7 @@
     <sheet name="Misc- steps" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -751,18 +752,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -770,10 +759,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1068,7 +1069,7 @@
   <dimension ref="A2:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,381 +1100,381 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="13">
         <v>1</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="18"/>
+      <c r="E3" s="14"/>
       <c r="I3" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="13">
         <v>2</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="14"/>
       <c r="I4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="13">
         <v>3</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="14"/>
       <c r="I5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="13">
         <v>4</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="18"/>
+      <c r="E6" s="14"/>
       <c r="I6" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="13">
         <v>5</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="18"/>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="13">
         <v>6</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="13">
         <v>7</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="13">
         <v>8</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="14"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="18">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="13">
         <v>9</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="18"/>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="18">
+      <c r="A12" s="19"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="14">
         <v>10</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="E12" s="18"/>
+      <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16" t="s">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="14">
         <v>10</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="18"/>
+      <c r="E14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="18">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="14">
         <v>11</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="18"/>
+      <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="18">
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="14">
         <v>12</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="18"/>
+      <c r="E16" s="14"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="18">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="14">
         <v>13</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="18"/>
+      <c r="E17" s="14"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16" t="s">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="14">
         <v>14</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="18"/>
+      <c r="E19" s="14"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="18">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="14">
         <v>15</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="18"/>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="18">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="14">
         <v>16</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="18"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="18">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="14">
         <v>17</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="14"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="18">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="14">
         <v>18</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="18">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="14">
         <v>19</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E24" s="18"/>
+      <c r="E24" s="14"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="18">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="14">
         <v>20</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E25" s="18"/>
+      <c r="E25" s="14"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="21" t="s">
+      <c r="A27" s="19"/>
+      <c r="B27" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="14">
         <v>21</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E27" s="18"/>
+      <c r="E27" s="14"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="18">
+      <c r="A28" s="19"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="14">
         <v>22</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E28" s="18"/>
+      <c r="E28" s="14"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
     </row>
     <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="18" t="s">
+      <c r="A30" s="19"/>
+      <c r="B30" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="14">
         <v>23</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="17" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14">
         <v>24</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="14" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14">
         <v>25</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="14" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14">
         <v>26</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="14" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18" t="s">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="14">
         <v>27</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="E35" s="18"/>
+      <c r="E35" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1517,7 +1518,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
       <c r="B2">
@@ -1531,7 +1532,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="20"/>
       <c r="B3">
         <v>2</v>
       </c>
@@ -1543,7 +1544,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="20"/>
       <c r="B4">
         <v>3</v>
       </c>
@@ -1552,7 +1553,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="20"/>
       <c r="B5">
         <v>4</v>
       </c>
@@ -1564,7 +1565,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="20"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -1573,7 +1574,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="20"/>
       <c r="B7">
         <v>6</v>
       </c>
@@ -1582,7 +1583,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="20"/>
       <c r="B8">
         <v>7</v>
       </c>
@@ -1594,7 +1595,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="20"/>
       <c r="B9">
         <v>8</v>
       </c>
@@ -1606,7 +1607,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
+      <c r="A10" s="20"/>
       <c r="B10">
         <v>9</v>
       </c>
@@ -1624,7 +1625,7 @@
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="A12" s="20">
         <v>2</v>
       </c>
       <c r="B12">
@@ -1638,7 +1639,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="20"/>
       <c r="B13">
         <v>2</v>
       </c>
@@ -1650,7 +1651,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="20"/>
       <c r="B14">
         <v>3</v>
       </c>
@@ -1659,7 +1660,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="20"/>
       <c r="B15">
         <v>4</v>
       </c>
@@ -1677,7 +1678,7 @@
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="A17" s="20">
         <v>3</v>
       </c>
       <c r="B17">
@@ -1691,7 +1692,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+      <c r="A18" s="20"/>
       <c r="B18">
         <v>2</v>
       </c>
@@ -1703,7 +1704,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="20"/>
       <c r="B19">
         <v>3</v>
       </c>
@@ -1712,7 +1713,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="A20" s="20"/>
       <c r="B20">
         <v>4</v>
       </c>
@@ -1730,7 +1731,7 @@
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
+      <c r="A22" s="20">
         <v>4</v>
       </c>
       <c r="B22">
@@ -1744,7 +1745,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+      <c r="A23" s="20"/>
       <c r="B23">
         <v>2</v>
       </c>
@@ -1756,7 +1757,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
+      <c r="A24" s="20"/>
       <c r="B24">
         <v>3</v>
       </c>
@@ -1765,7 +1766,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
+      <c r="A25" s="20"/>
       <c r="B25">
         <v>4</v>
       </c>
@@ -1777,7 +1778,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
+      <c r="A26" s="20"/>
       <c r="B26">
         <v>5</v>
       </c>
@@ -1795,7 +1796,7 @@
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="A28" s="20">
         <v>5</v>
       </c>
       <c r="B28">
@@ -1809,7 +1810,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
+      <c r="A29" s="20"/>
       <c r="B29">
         <v>2</v>
       </c>
@@ -1821,7 +1822,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
+      <c r="A30" s="20"/>
       <c r="B30">
         <v>3</v>
       </c>
@@ -1830,7 +1831,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
+      <c r="A31" s="20"/>
       <c r="B31">
         <v>4</v>
       </c>
@@ -1839,7 +1840,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
+      <c r="A32" s="20"/>
       <c r="B32">
         <v>5</v>
       </c>
@@ -1857,7 +1858,7 @@
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+      <c r="A34" s="20">
         <v>6</v>
       </c>
       <c r="B34">
@@ -1871,7 +1872,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
+      <c r="A35" s="20"/>
       <c r="B35">
         <v>2</v>
       </c>
@@ -1883,7 +1884,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
+      <c r="A36" s="20"/>
       <c r="B36">
         <v>3</v>
       </c>
@@ -1892,7 +1893,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+      <c r="A37" s="20"/>
       <c r="B37">
         <v>4</v>
       </c>
@@ -1901,7 +1902,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
+      <c r="A38" s="20"/>
       <c r="B38">
         <v>5</v>
       </c>
@@ -1919,7 +1920,7 @@
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="15">
+      <c r="A40" s="20">
         <v>7</v>
       </c>
       <c r="B40">
@@ -1933,7 +1934,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
+      <c r="A41" s="20"/>
       <c r="B41">
         <v>2</v>
       </c>
@@ -1945,7 +1946,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
+      <c r="A42" s="20"/>
       <c r="B42">
         <v>3</v>
       </c>
@@ -1954,7 +1955,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
+      <c r="A43" s="20"/>
       <c r="B43">
         <v>4</v>
       </c>
@@ -1963,7 +1964,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
+      <c r="A44" s="20"/>
       <c r="B44">
         <v>5</v>
       </c>
@@ -1981,7 +1982,7 @@
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="15">
+      <c r="A46" s="20">
         <v>8</v>
       </c>
       <c r="B46">
@@ -1995,7 +1996,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
+      <c r="A47" s="20"/>
       <c r="B47">
         <v>2</v>
       </c>
@@ -2007,7 +2008,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
+      <c r="A48" s="20"/>
       <c r="B48">
         <v>3</v>
       </c>
@@ -2019,7 +2020,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
+      <c r="A49" s="20"/>
       <c r="B49">
         <v>4</v>
       </c>
@@ -2028,7 +2029,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
+      <c r="A50" s="20"/>
       <c r="B50">
         <v>5</v>
       </c>
@@ -2040,7 +2041,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
+      <c r="A51" s="20"/>
       <c r="B51">
         <v>6</v>
       </c>
@@ -2056,7 +2057,7 @@
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="14">
+      <c r="A53" s="21">
         <v>9</v>
       </c>
       <c r="B53">
@@ -2070,7 +2071,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
+      <c r="A54" s="21"/>
       <c r="B54">
         <v>2</v>
       </c>
@@ -2082,7 +2083,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
+      <c r="A55" s="21"/>
       <c r="B55">
         <v>3</v>
       </c>
@@ -2094,7 +2095,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
+      <c r="A56" s="21"/>
       <c r="B56">
         <v>4</v>
       </c>
@@ -2103,7 +2104,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="21"/>
       <c r="B57">
         <v>5</v>
       </c>
@@ -2115,7 +2116,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
+      <c r="A58" s="21"/>
       <c r="B58">
         <v>6</v>
       </c>
@@ -2131,7 +2132,7 @@
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="14">
+      <c r="A60" s="21">
         <v>10</v>
       </c>
       <c r="B60">
@@ -2145,7 +2146,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
+      <c r="A61" s="21"/>
       <c r="B61">
         <v>2</v>
       </c>
@@ -2157,7 +2158,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="21"/>
       <c r="B62">
         <v>3</v>
       </c>
@@ -2166,7 +2167,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+      <c r="A63" s="21"/>
       <c r="B63">
         <v>4</v>
       </c>
@@ -2178,7 +2179,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="21"/>
       <c r="B64">
         <v>5</v>
       </c>
@@ -2187,7 +2188,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
+      <c r="A65" s="21"/>
       <c r="B65">
         <v>6</v>
       </c>
@@ -2196,7 +2197,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
+      <c r="A66" s="21"/>
       <c r="B66">
         <v>7</v>
       </c>
@@ -2205,7 +2206,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
+      <c r="A67" s="21"/>
       <c r="B67">
         <v>8</v>
       </c>
@@ -2214,7 +2215,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2264,7 +2265,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="21">
         <v>10</v>
       </c>
       <c r="B2">
@@ -2278,7 +2279,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="21"/>
       <c r="B3">
         <v>2</v>
       </c>
@@ -2290,7 +2291,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="21"/>
       <c r="B4">
         <v>3</v>
       </c>
@@ -2299,7 +2300,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="A5" s="21"/>
       <c r="B5">
         <v>4</v>
       </c>
@@ -2308,7 +2309,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="21"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -2317,7 +2318,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="21"/>
       <c r="B7">
         <v>6</v>
       </c>
@@ -2326,7 +2327,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="21"/>
       <c r="B8">
         <v>7</v>
       </c>
@@ -2335,7 +2336,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="21"/>
       <c r="B9">
         <v>8</v>
       </c>
@@ -2344,7 +2345,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="21"/>
       <c r="B10">
         <v>9</v>
       </c>
@@ -2353,7 +2354,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="21"/>
       <c r="B11">
         <v>10</v>
       </c>
@@ -2371,7 +2372,7 @@
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="A13" s="21">
         <v>11</v>
       </c>
       <c r="B13">
@@ -2385,7 +2386,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="21"/>
       <c r="B14">
         <v>2</v>
       </c>
@@ -2397,7 +2398,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="21"/>
       <c r="B15">
         <v>3</v>
       </c>
@@ -2406,7 +2407,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+      <c r="A16" s="21"/>
       <c r="B16">
         <v>4</v>
       </c>
@@ -2415,7 +2416,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="21"/>
       <c r="B17">
         <v>5</v>
       </c>
@@ -2424,7 +2425,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="21"/>
       <c r="B18">
         <v>6</v>
       </c>
@@ -2433,7 +2434,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="21"/>
       <c r="B19">
         <v>7</v>
       </c>
@@ -2442,7 +2443,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="21"/>
       <c r="B20">
         <v>8</v>
       </c>
@@ -2451,7 +2452,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="A21" s="21"/>
       <c r="B21">
         <v>9</v>
       </c>
@@ -2460,7 +2461,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="21"/>
       <c r="B22">
         <v>10</v>
       </c>
@@ -2478,7 +2479,7 @@
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
+      <c r="A24" s="21">
         <v>12</v>
       </c>
       <c r="B24">
@@ -2492,7 +2493,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="21"/>
       <c r="B25">
         <v>2</v>
       </c>
@@ -2504,7 +2505,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+      <c r="A26" s="21"/>
       <c r="B26">
         <v>3</v>
       </c>
@@ -2513,7 +2514,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="21"/>
       <c r="B27">
         <v>4</v>
       </c>
@@ -2522,7 +2523,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="21"/>
       <c r="B28">
         <v>5</v>
       </c>
@@ -2531,7 +2532,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="21"/>
       <c r="B29">
         <v>6</v>
       </c>
@@ -2540,7 +2541,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="21"/>
       <c r="B30">
         <v>7</v>
       </c>
@@ -2549,7 +2550,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="21"/>
       <c r="B31">
         <v>8</v>
       </c>
@@ -2558,7 +2559,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="21"/>
       <c r="B32">
         <v>9</v>
       </c>
@@ -2567,7 +2568,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="21"/>
       <c r="B33">
         <v>10</v>
       </c>
@@ -2624,7 +2625,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="21">
         <v>14</v>
       </c>
       <c r="B2">
@@ -2635,7 +2636,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="21"/>
       <c r="B3">
         <v>2</v>
       </c>
@@ -2644,7 +2645,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="100.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="21"/>
       <c r="B4">
         <v>3</v>
       </c>
@@ -2656,7 +2657,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="A5" s="21"/>
       <c r="B5">
         <v>4</v>
       </c>
@@ -2665,7 +2666,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="21"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -2677,7 +2678,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="21"/>
       <c r="B7">
         <v>6</v>
       </c>
@@ -2686,7 +2687,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="21"/>
       <c r="B8">
         <v>7</v>
       </c>
@@ -2698,7 +2699,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="21"/>
       <c r="B9">
         <v>8</v>
       </c>
@@ -2707,7 +2708,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="21"/>
       <c r="B10">
         <v>9</v>
       </c>
@@ -2719,7 +2720,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="21"/>
       <c r="B11">
         <v>10</v>
       </c>
@@ -2731,7 +2732,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="21"/>
       <c r="B12">
         <v>11</v>
       </c>
@@ -2740,7 +2741,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="21"/>
       <c r="B13">
         <v>12</v>
       </c>
@@ -2752,7 +2753,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="21"/>
       <c r="B14">
         <v>13</v>
       </c>
@@ -2761,7 +2762,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="21"/>
       <c r="B15">
         <v>14</v>
       </c>
@@ -2770,7 +2771,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+      <c r="A16" s="21"/>
       <c r="B16">
         <v>15</v>
       </c>
@@ -2788,7 +2789,7 @@
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
+      <c r="A18" s="21">
         <v>15</v>
       </c>
       <c r="B18">
@@ -2799,7 +2800,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="21"/>
       <c r="B19">
         <v>2</v>
       </c>
@@ -2808,7 +2809,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="21"/>
       <c r="B20">
         <v>3</v>
       </c>
@@ -2826,7 +2827,7 @@
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
+      <c r="A22" s="21">
         <v>16</v>
       </c>
       <c r="B22">
@@ -2837,7 +2838,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="21"/>
       <c r="B23">
         <v>2</v>
       </c>
@@ -2846,7 +2847,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="21"/>
       <c r="B24">
         <v>3</v>
       </c>
@@ -2864,7 +2865,7 @@
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
+      <c r="A26" s="21">
         <v>17</v>
       </c>
       <c r="B26">
@@ -2875,7 +2876,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="21"/>
       <c r="B27">
         <v>2</v>
       </c>
@@ -2884,7 +2885,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="21"/>
       <c r="B28">
         <v>3</v>
       </c>
@@ -2902,7 +2903,7 @@
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
+      <c r="A30" s="21">
         <v>18</v>
       </c>
       <c r="B30">
@@ -2913,7 +2914,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="21"/>
       <c r="B31">
         <v>2</v>
       </c>
@@ -2922,7 +2923,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="21"/>
       <c r="B32">
         <v>3</v>
       </c>
@@ -2940,7 +2941,7 @@
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
+      <c r="A34" s="21">
         <v>19</v>
       </c>
       <c r="B34">
@@ -2951,7 +2952,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="21"/>
       <c r="B35">
         <v>2</v>
       </c>
@@ -2960,7 +2961,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
+      <c r="A36" s="21"/>
       <c r="B36">
         <v>3</v>
       </c>
@@ -2969,7 +2970,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+      <c r="A37" s="21"/>
       <c r="B37">
         <v>4</v>
       </c>
@@ -2978,7 +2979,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="21"/>
       <c r="B38">
         <v>5</v>
       </c>
@@ -2987,7 +2988,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="21"/>
       <c r="B39">
         <v>6</v>
       </c>
@@ -2996,7 +2997,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="21"/>
       <c r="B40">
         <v>7</v>
       </c>
@@ -3005,7 +3006,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="21"/>
       <c r="B41">
         <v>8</v>
       </c>
@@ -3017,7 +3018,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="21"/>
       <c r="B42">
         <v>9</v>
       </c>
@@ -3029,7 +3030,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="21"/>
       <c r="B43">
         <v>10</v>
       </c>
@@ -3041,7 +3042,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="21"/>
       <c r="B44">
         <v>11</v>
       </c>
@@ -3059,7 +3060,7 @@
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="14">
+      <c r="A46" s="21">
         <v>20</v>
       </c>
       <c r="B46">
@@ -3070,7 +3071,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="21"/>
       <c r="B47">
         <v>2</v>
       </c>
@@ -3079,7 +3080,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="A48" s="21"/>
       <c r="B48">
         <v>3</v>
       </c>
@@ -3088,7 +3089,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="21"/>
       <c r="B49">
         <v>4</v>
       </c>
@@ -3097,7 +3098,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="A50" s="21"/>
       <c r="B50">
         <v>5</v>
       </c>
@@ -3244,7 +3245,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="21">
         <v>23</v>
       </c>
       <c r="B2">
@@ -3255,7 +3256,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="21"/>
       <c r="B3">
         <v>2</v>
       </c>
@@ -3267,7 +3268,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="21"/>
       <c r="B4">
         <v>3</v>
       </c>
@@ -3279,7 +3280,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="A5" s="21"/>
       <c r="B5">
         <v>4</v>
       </c>
@@ -3291,7 +3292,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="21"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -3303,7 +3304,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="21"/>
       <c r="B7">
         <v>6</v>
       </c>
@@ -3315,7 +3316,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="21"/>
       <c r="B8">
         <v>7</v>
       </c>
@@ -3327,7 +3328,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="21"/>
       <c r="B9">
         <v>8</v>
       </c>
@@ -3345,7 +3346,7 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="21">
         <v>24</v>
       </c>
       <c r="B11">
@@ -3359,7 +3360,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="21"/>
       <c r="B12">
         <v>2</v>
       </c>
@@ -3371,7 +3372,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="21"/>
       <c r="B13">
         <v>3</v>
       </c>
@@ -3383,7 +3384,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="21"/>
       <c r="B14">
         <v>4</v>
       </c>
@@ -3392,7 +3393,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="21"/>
       <c r="B15">
         <v>5</v>
       </c>
@@ -3401,7 +3402,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+      <c r="A16" s="21"/>
       <c r="B16">
         <v>6</v>
       </c>
@@ -3413,7 +3414,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="21"/>
       <c r="B17">
         <v>7</v>
       </c>
@@ -3425,7 +3426,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="21"/>
       <c r="B18">
         <v>8</v>
       </c>
@@ -3437,7 +3438,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="21"/>
       <c r="B19">
         <v>9</v>
       </c>
@@ -3452,7 +3453,7 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
+      <c r="A21" s="21">
         <v>25</v>
       </c>
       <c r="B21">
@@ -3466,7 +3467,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="21"/>
       <c r="B22">
         <v>2</v>
       </c>
@@ -3475,7 +3476,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="21"/>
       <c r="B23">
         <v>3</v>
       </c>
@@ -3484,7 +3485,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="21"/>
       <c r="B24">
         <v>4</v>
       </c>
@@ -3493,7 +3494,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="21"/>
       <c r="B25">
         <v>5</v>
       </c>
@@ -3505,7 +3506,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+      <c r="A26" s="21"/>
       <c r="B26">
         <v>6</v>
       </c>
@@ -3514,7 +3515,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="21"/>
       <c r="B27">
         <v>7</v>
       </c>
@@ -3532,7 +3533,7 @@
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
+      <c r="A29" s="21">
         <v>26</v>
       </c>
       <c r="B29">
@@ -3546,7 +3547,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="21"/>
       <c r="B30">
         <v>2</v>
       </c>
@@ -3555,7 +3556,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="21"/>
       <c r="B31">
         <v>3</v>
       </c>
@@ -3564,7 +3565,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="21"/>
       <c r="B32">
         <v>4</v>
       </c>
@@ -3573,7 +3574,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="21"/>
       <c r="B33">
         <v>5</v>
       </c>
@@ -3632,7 +3633,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="22">
         <v>27</v>
       </c>
       <c r="B2">
@@ -3643,7 +3644,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
+      <c r="A3" s="22"/>
       <c r="B3">
         <v>2</v>
       </c>

</xml_diff>